<commit_message>
Import user, items, warehouse, uom, department
</commit_message>
<xml_diff>
--- a/assets/excel/UoM.xlsx
+++ b/assets/excel/UoM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Import Data UoM</t>
+  </si>
+  <si>
+    <t>satuduatiga</t>
   </si>
 </sst>
 </file>
@@ -107,14 +110,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,32 +405,36 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="A3:B13"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
+      <c r="A3" s="4">
+        <v>123</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4"/>

</xml_diff>